<commit_message>
CORELIMS-98 - production addition of F3
</commit_message>
<xml_diff>
--- a/output/freezer_03_shelf1/c3_exceldata.xlsx
+++ b/output/freezer_03_shelf1/c3_exceldata.xlsx
@@ -28,7 +28,7 @@
     <t>F3-S1-R1-D1</t>
   </si>
   <si>
-    <t>RCK89</t>
+    <t>RCK99</t>
   </si>
   <si>
     <t>F3-S1-R1-D2</t>
@@ -52,7 +52,7 @@
     <t>F3-S1-R2-D1</t>
   </si>
   <si>
-    <t>RCK90</t>
+    <t>RCK100</t>
   </si>
   <si>
     <t>F3-S1-R2-D2</t>
@@ -76,7 +76,7 @@
     <t>F3-S1-R3-D1</t>
   </si>
   <si>
-    <t>RCK91</t>
+    <t>RCK101</t>
   </si>
   <si>
     <t>F3-S1-R3-D2</t>
@@ -100,7 +100,7 @@
     <t>F3-S1-R4-D1</t>
   </si>
   <si>
-    <t>RCK92</t>
+    <t>RCK102</t>
   </si>
   <si>
     <t>F3-S1-R4-D2</t>
@@ -124,7 +124,7 @@
     <t>F3-S1-R5-D1</t>
   </si>
   <si>
-    <t>RCK93</t>
+    <t>RCK103</t>
   </si>
   <si>
     <t>F3-S1-R5-D2</t>
@@ -148,7 +148,7 @@
     <t>F3-S1-R6-D1</t>
   </si>
   <si>
-    <t>RCK94</t>
+    <t>RCK104</t>
   </si>
   <si>
     <t>F3-S1-R6-D2</t>

</xml_diff>